<commit_message>
Exclude participants with over 4 majors
</commit_message>
<xml_diff>
--- a/output/unstdpearson_correlations.xlsx
+++ b/output/unstdpearson_correlations.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">Variable</t>
   </si>
@@ -47,7 +47,7 @@
     <t xml:space="preserve">2. interest.all</t>
   </si>
   <si>
-    <t xml:space="preserve">6.03</t>
+    <t xml:space="preserve">6.02</t>
   </si>
   <si>
     <t xml:space="preserve">0.73</t>
@@ -74,13 +74,10 @@
     <t xml:space="preserve">4. dd.id.all</t>
   </si>
   <si>
-    <t xml:space="preserve">6.26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.82</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.65**</t>
+    <t xml:space="preserve">0.81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.66**</t>
   </si>
   <si>
     <t xml:space="preserve">.80**</t>
@@ -531,16 +528,16 @@
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>17</v>

</xml_diff>